<commit_message>
Kind -> Index로 이름 수정
</commit_message>
<xml_diff>
--- a/XLSX/MonsterGroupTable.xlsx
+++ b/XLSX/MonsterGroupTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CProject\SProject\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD38A75-6122-40F0-B5DB-3201141D8E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525C3B0D-01FF-471B-A6E1-8ED85703A624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29655" yWindow="4335" windowWidth="21600" windowHeight="12645" xr2:uid="{634E5D1F-E6A6-48B1-B744-D317D5276317}"/>
+    <workbookView xWindow="36015" yWindow="3165" windowWidth="17700" windowHeight="11385" xr2:uid="{634E5D1F-E6A6-48B1-B744-D317D5276317}"/>
   </bookViews>
   <sheets>
     <sheet name="!MonsterGroup" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Kind</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -69,6 +69,10 @@
   </si>
   <si>
     <t>;해당 그룹에 속할 몬스터 수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -478,7 +482,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -491,7 +495,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -542,7 +546,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1001</v>
@@ -559,7 +563,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>1001</v>
@@ -576,7 +580,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>1001</v>
@@ -593,7 +597,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>1001</v>
@@ -610,7 +614,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>1001</v>

</xml_diff>